<commit_message>
corrected 40096184 to reflect fix cleared crash
</commit_message>
<xml_diff>
--- a/runs/arvo_codex_experiments.xlsx
+++ b/runs/arvo_codex_experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e26497900af22851/Documents/Education/ML Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apruf\repos\ARVO-Codex-Logger\runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{23C45E14-39F8-4554-BD2A-3DCC2F8C3FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDFAE5C1-0343-41D3-A510-B104C5927EBF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB980D0-CF72-4830-BA82-E5ED203439A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{CA653102-D0FF-42E2-93AB-EE7AAFF2C012}"/>
   </bookViews>
@@ -95,13 +95,13 @@
     <t>final_patch_gt_variation</t>
   </si>
   <si>
-    <t>Patched different file than GT, but crash still cleared. Cost spiked in time and tokens.</t>
-  </si>
-  <si>
     <t>patch2 context included GT fixed files and approx line numbers</t>
   </si>
   <si>
     <t>1766121970, 1767071807</t>
+  </si>
+  <si>
+    <t>Patched different file than GT, but crash still cleared.</t>
   </si>
 </sst>
 </file>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78776FF9-70DB-40C5-AB34-5AC146E95C32}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -668,7 +668,7 @@
         <v>40096184</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1078.17287445068</v>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
@@ -742,13 +742,13 @@
         <v>8041461</v>
       </c>
       <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
         <v>20</v>
-      </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>